<commit_message>
Created R-friendly versions of data files
</commit_message>
<xml_diff>
--- a/Data/Biggest_Loser.xlsx
+++ b/Data/Biggest_Loser.xlsx
@@ -1,21 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://webmailbyui-my.sharepoint.com/personal/drp36_byui_edu/Documents/221/Course_Files/BYUI_M221_Book/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Downloads\Temp data folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DEFC8335-E8FB-47B4-89A0-63E577B6C38D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896957ED-212E-4ADE-8DDD-4F5333E65CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8580" yWindow="1320" windowWidth="19875" windowHeight="13980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -442,13 +453,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K278"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -483,7 +492,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -518,7 +527,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -553,7 +562,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -588,7 +597,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -623,7 +632,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -658,7 +667,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -693,7 +702,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -728,7 +737,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -763,7 +772,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -798,7 +807,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -833,7 +842,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -868,7 +877,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -903,7 +912,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -938,7 +947,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -973,7 +982,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1008,7 +1017,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1043,7 +1052,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -1078,7 +1087,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -1113,7 +1122,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1148,7 +1157,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -1183,7 +1192,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -1218,7 +1227,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1253,7 +1262,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -1288,7 +1297,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -1323,7 +1332,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -1358,7 +1367,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -1393,7 +1402,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -1428,7 +1437,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -1463,7 +1472,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -1498,7 +1507,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -1533,7 +1542,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>13</v>
       </c>
@@ -1568,7 +1577,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -1603,7 +1612,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -1638,7 +1647,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -1673,7 +1682,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>13</v>
       </c>
@@ -1708,7 +1717,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>13</v>
       </c>
@@ -1743,7 +1752,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>13</v>
       </c>
@@ -1778,7 +1787,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -1813,7 +1822,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -1848,7 +1857,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>13</v>
       </c>
@@ -1883,7 +1892,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>13</v>
       </c>
@@ -1918,7 +1927,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -1953,7 +1962,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>9</v>
       </c>
@@ -1988,7 +1997,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>13</v>
       </c>
@@ -2023,7 +2032,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>9</v>
       </c>
@@ -2058,7 +2067,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>9</v>
       </c>
@@ -2093,7 +2102,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>13</v>
       </c>
@@ -2128,7 +2137,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>13</v>
       </c>
@@ -2163,7 +2172,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>9</v>
       </c>
@@ -2198,7 +2207,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>13</v>
       </c>
@@ -2233,7 +2242,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>9</v>
       </c>
@@ -2268,7 +2277,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>9</v>
       </c>
@@ -2303,7 +2312,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>9</v>
       </c>
@@ -2338,7 +2347,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>13</v>
       </c>
@@ -2373,7 +2382,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>13</v>
       </c>
@@ -2408,7 +2417,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>13</v>
       </c>
@@ -2443,7 +2452,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>13</v>
       </c>
@@ -2478,7 +2487,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>9</v>
       </c>
@@ -2513,7 +2522,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>9</v>
       </c>
@@ -2548,7 +2557,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>9</v>
       </c>
@@ -2583,7 +2592,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>13</v>
       </c>
@@ -2618,7 +2627,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>13</v>
       </c>
@@ -2653,7 +2662,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>9</v>
       </c>
@@ -2688,7 +2697,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>13</v>
       </c>
@@ -2723,7 +2732,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>9</v>
       </c>
@@ -2758,7 +2767,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>9</v>
       </c>
@@ -2793,7 +2802,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>13</v>
       </c>
@@ -2828,7 +2837,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>13</v>
       </c>
@@ -2863,7 +2872,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>9</v>
       </c>
@@ -2898,7 +2907,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>13</v>
       </c>
@@ -2933,7 +2942,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>13</v>
       </c>
@@ -2968,7 +2977,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>9</v>
       </c>
@@ -3003,7 +3012,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>9</v>
       </c>
@@ -3038,7 +3047,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>9</v>
       </c>
@@ -3073,7 +3082,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>13</v>
       </c>
@@ -3108,7 +3117,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>13</v>
       </c>
@@ -3143,7 +3152,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>9</v>
       </c>
@@ -3178,7 +3187,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>9</v>
       </c>
@@ -3213,7 +3222,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>9</v>
       </c>
@@ -3248,7 +3257,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>9</v>
       </c>
@@ -3283,7 +3292,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>13</v>
       </c>
@@ -3318,7 +3327,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>9</v>
       </c>
@@ -3353,7 +3362,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>13</v>
       </c>
@@ -3388,7 +3397,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>9</v>
       </c>
@@ -3423,7 +3432,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>13</v>
       </c>
@@ -3458,7 +3467,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>9</v>
       </c>
@@ -3493,7 +3502,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>13</v>
       </c>
@@ -3528,7 +3537,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>13</v>
       </c>
@@ -3563,7 +3572,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>9</v>
       </c>
@@ -3598,7 +3607,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>9</v>
       </c>
@@ -3633,7 +3642,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>13</v>
       </c>
@@ -3668,7 +3677,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>13</v>
       </c>
@@ -3703,7 +3712,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>13</v>
       </c>
@@ -3738,7 +3747,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>9</v>
       </c>
@@ -3773,7 +3782,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>13</v>
       </c>
@@ -3808,7 +3817,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>9</v>
       </c>
@@ -3843,7 +3852,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>13</v>
       </c>
@@ -3878,7 +3887,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>13</v>
       </c>
@@ -3913,7 +3922,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>13</v>
       </c>
@@ -3948,7 +3957,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>9</v>
       </c>
@@ -3983,7 +3992,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>13</v>
       </c>
@@ -4018,7 +4027,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>9</v>
       </c>
@@ -4053,7 +4062,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>9</v>
       </c>
@@ -4088,7 +4097,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>9</v>
       </c>
@@ -4123,7 +4132,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>13</v>
       </c>
@@ -4158,7 +4167,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>9</v>
       </c>
@@ -4193,7 +4202,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>9</v>
       </c>
@@ -4228,7 +4237,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>9</v>
       </c>
@@ -4263,7 +4272,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>9</v>
       </c>
@@ -4298,7 +4307,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>9</v>
       </c>
@@ -4333,7 +4342,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>13</v>
       </c>
@@ -4368,7 +4377,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>13</v>
       </c>
@@ -4403,7 +4412,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>9</v>
       </c>
@@ -4438,7 +4447,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>9</v>
       </c>
@@ -4473,7 +4482,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>13</v>
       </c>
@@ -4508,7 +4517,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>9</v>
       </c>
@@ -4543,7 +4552,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>13</v>
       </c>
@@ -4578,7 +4587,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>9</v>
       </c>
@@ -4613,7 +4622,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>9</v>
       </c>
@@ -4648,7 +4657,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>13</v>
       </c>
@@ -4683,7 +4692,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>9</v>
       </c>
@@ -4718,7 +4727,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>13</v>
       </c>
@@ -4753,7 +4762,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>9</v>
       </c>
@@ -4788,7 +4797,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>9</v>
       </c>
@@ -4823,7 +4832,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>13</v>
       </c>
@@ -4858,7 +4867,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>13</v>
       </c>
@@ -4893,7 +4902,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>13</v>
       </c>
@@ -4928,7 +4937,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>9</v>
       </c>
@@ -4963,7 +4972,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>13</v>
       </c>
@@ -4998,7 +5007,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>13</v>
       </c>
@@ -5033,7 +5042,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>9</v>
       </c>
@@ -5068,7 +5077,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>13</v>
       </c>
@@ -5103,7 +5112,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>9</v>
       </c>
@@ -5138,7 +5147,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>9</v>
       </c>
@@ -5173,7 +5182,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>13</v>
       </c>
@@ -5208,7 +5217,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>9</v>
       </c>
@@ -5243,7 +5252,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>13</v>
       </c>
@@ -5278,7 +5287,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>13</v>
       </c>
@@ -5313,7 +5322,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>13</v>
       </c>
@@ -5348,7 +5357,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>13</v>
       </c>
@@ -5383,7 +5392,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>9</v>
       </c>
@@ -5418,7 +5427,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>13</v>
       </c>
@@ -5453,7 +5462,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>9</v>
       </c>
@@ -5488,7 +5497,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>9</v>
       </c>
@@ -5523,7 +5532,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>9</v>
       </c>
@@ -5558,7 +5567,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>9</v>
       </c>
@@ -5593,7 +5602,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>9</v>
       </c>
@@ -5628,7 +5637,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>9</v>
       </c>
@@ -5663,7 +5672,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>13</v>
       </c>
@@ -5698,7 +5707,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>9</v>
       </c>
@@ -5733,7 +5742,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>9</v>
       </c>
@@ -5768,7 +5777,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>13</v>
       </c>
@@ -5803,7 +5812,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>13</v>
       </c>
@@ -5838,7 +5847,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>9</v>
       </c>
@@ -5873,7 +5882,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>13</v>
       </c>
@@ -5908,7 +5917,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>9</v>
       </c>
@@ -5943,7 +5952,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>13</v>
       </c>
@@ -5978,7 +5987,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>9</v>
       </c>
@@ -6013,7 +6022,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>13</v>
       </c>
@@ -6048,7 +6057,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>9</v>
       </c>
@@ -6083,7 +6092,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>13</v>
       </c>
@@ -6118,7 +6127,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>13</v>
       </c>
@@ -6153,7 +6162,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>9</v>
       </c>
@@ -6188,7 +6197,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>9</v>
       </c>
@@ -6223,7 +6232,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>13</v>
       </c>
@@ -6258,7 +6267,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>9</v>
       </c>
@@ -6293,7 +6302,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>9</v>
       </c>
@@ -6328,7 +6337,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>9</v>
       </c>
@@ -6363,7 +6372,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>9</v>
       </c>
@@ -6398,7 +6407,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>13</v>
       </c>
@@ -6433,7 +6442,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>9</v>
       </c>
@@ -6468,7 +6477,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>9</v>
       </c>
@@ -6503,7 +6512,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>13</v>
       </c>
@@ -6538,7 +6547,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>9</v>
       </c>
@@ -6573,7 +6582,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>13</v>
       </c>
@@ -6608,7 +6617,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>13</v>
       </c>
@@ -6643,7 +6652,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>13</v>
       </c>
@@ -6678,7 +6687,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>9</v>
       </c>
@@ -6713,7 +6722,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>9</v>
       </c>
@@ -6748,7 +6757,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>13</v>
       </c>
@@ -6783,7 +6792,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>13</v>
       </c>
@@ -6818,7 +6827,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>13</v>
       </c>
@@ -6853,7 +6862,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>9</v>
       </c>
@@ -6888,7 +6897,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>13</v>
       </c>
@@ -6923,7 +6932,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>9</v>
       </c>
@@ -6958,7 +6967,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>9</v>
       </c>
@@ -6993,7 +7002,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>13</v>
       </c>
@@ -7028,7 +7037,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>13</v>
       </c>
@@ -7063,7 +7072,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>13</v>
       </c>
@@ -7098,7 +7107,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>9</v>
       </c>
@@ -7133,7 +7142,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>13</v>
       </c>
@@ -7168,7 +7177,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>9</v>
       </c>
@@ -7203,7 +7212,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>13</v>
       </c>
@@ -7238,7 +7247,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>13</v>
       </c>
@@ -7273,7 +7282,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>9</v>
       </c>
@@ -7308,7 +7317,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>9</v>
       </c>
@@ -7343,7 +7352,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>13</v>
       </c>
@@ -7378,7 +7387,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>9</v>
       </c>
@@ -7413,7 +7422,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>13</v>
       </c>
@@ -7448,7 +7457,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>13</v>
       </c>
@@ -7483,7 +7492,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>9</v>
       </c>
@@ -7518,7 +7527,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>13</v>
       </c>
@@ -7553,7 +7562,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>9</v>
       </c>
@@ -7588,7 +7597,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>9</v>
       </c>
@@ -7623,7 +7632,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>9</v>
       </c>
@@ -7658,7 +7667,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>9</v>
       </c>
@@ -7693,7 +7702,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>13</v>
       </c>
@@ -7728,7 +7737,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>9</v>
       </c>
@@ -7763,7 +7772,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>13</v>
       </c>
@@ -7798,7 +7807,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>9</v>
       </c>
@@ -7833,7 +7842,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>9</v>
       </c>
@@ -7868,7 +7877,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>9</v>
       </c>
@@ -7903,7 +7912,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>13</v>
       </c>
@@ -7938,7 +7947,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>9</v>
       </c>
@@ -7973,7 +7982,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>13</v>
       </c>
@@ -8008,7 +8017,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>13</v>
       </c>
@@ -8043,7 +8052,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>9</v>
       </c>
@@ -8078,7 +8087,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>9</v>
       </c>
@@ -8113,7 +8122,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>13</v>
       </c>
@@ -8148,7 +8157,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>9</v>
       </c>
@@ -8183,7 +8192,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>9</v>
       </c>
@@ -8218,7 +8227,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>13</v>
       </c>
@@ -8253,7 +8262,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>13</v>
       </c>
@@ -8288,7 +8297,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>9</v>
       </c>
@@ -8323,7 +8332,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>13</v>
       </c>
@@ -8358,7 +8367,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>9</v>
       </c>
@@ -8393,7 +8402,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>9</v>
       </c>
@@ -8428,7 +8437,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>13</v>
       </c>
@@ -8463,7 +8472,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>9</v>
       </c>
@@ -8498,7 +8507,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>9</v>
       </c>
@@ -8533,7 +8542,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>13</v>
       </c>
@@ -8568,7 +8577,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>13</v>
       </c>
@@ -8603,7 +8612,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>9</v>
       </c>
@@ -8638,7 +8647,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>9</v>
       </c>
@@ -8673,7 +8682,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
         <v>13</v>
       </c>
@@ -8708,7 +8717,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>9</v>
       </c>
@@ -8743,7 +8752,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>13</v>
       </c>
@@ -8778,7 +8787,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>13</v>
       </c>
@@ -8813,7 +8822,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
         <v>13</v>
       </c>
@@ -8848,7 +8857,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
         <v>9</v>
       </c>
@@ -8883,7 +8892,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
         <v>13</v>
       </c>
@@ -8918,7 +8927,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>9</v>
       </c>
@@ -8953,7 +8962,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>13</v>
       </c>
@@ -8988,7 +8997,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="245" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
         <v>9</v>
       </c>
@@ -9023,7 +9032,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
         <v>13</v>
       </c>
@@ -9058,7 +9067,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="247" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
         <v>13</v>
       </c>
@@ -9093,7 +9102,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
         <v>9</v>
       </c>
@@ -9128,7 +9137,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="249" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
         <v>9</v>
       </c>
@@ -9163,7 +9172,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
         <v>13</v>
       </c>
@@ -9198,7 +9207,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
         <v>13</v>
       </c>
@@ -9233,7 +9242,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="252" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
         <v>9</v>
       </c>
@@ -9268,7 +9277,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="253" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
         <v>13</v>
       </c>
@@ -9303,7 +9312,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="254" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
         <v>13</v>
       </c>
@@ -9338,7 +9347,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="255" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>9</v>
       </c>
@@ -9373,7 +9382,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
         <v>9</v>
       </c>
@@ -9408,7 +9417,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="257" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
         <v>9</v>
       </c>
@@ -9443,7 +9452,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="258" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
         <v>9</v>
       </c>
@@ -9478,7 +9487,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="259" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
         <v>9</v>
       </c>
@@ -9513,7 +9522,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="260" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
         <v>13</v>
       </c>
@@ -9548,7 +9557,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="261" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
         <v>13</v>
       </c>
@@ -9583,7 +9592,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="262" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
         <v>13</v>
       </c>
@@ -9618,7 +9627,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="263" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>9</v>
       </c>
@@ -9653,7 +9662,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="264" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>9</v>
       </c>
@@ -9688,7 +9697,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="265" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
         <v>9</v>
       </c>
@@ -9723,7 +9732,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="266" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
         <v>13</v>
       </c>
@@ -9758,7 +9767,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="267" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
         <v>9</v>
       </c>
@@ -9793,7 +9802,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="268" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
         <v>9</v>
       </c>
@@ -9828,7 +9837,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="269" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>9</v>
       </c>
@@ -9863,7 +9872,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
         <v>13</v>
       </c>
@@ -9898,7 +9907,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="271" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
         <v>13</v>
       </c>
@@ -9933,7 +9942,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="272" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>9</v>
       </c>
@@ -9968,7 +9977,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>9</v>
       </c>
@@ -10003,7 +10012,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>9</v>
       </c>
@@ -10038,7 +10047,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>9</v>
       </c>
@@ -10073,7 +10082,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
         <v>13</v>
       </c>
@@ -10108,7 +10117,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
         <v>13</v>
       </c>
@@ -10143,7 +10152,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
         <v>13</v>
       </c>

</xml_diff>